<commit_message>
Implementación de remember y recall
</commit_message>
<xml_diff>
--- a/build/resources/test/Data/Data.xlsx
+++ b/build/resources/test/Data/Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Search</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Google Tv Hyundai Smart 43 Fhd Comando De Voz</t>
+  </si>
+  <si>
+    <t>Televisor JVC 50 Pulgadas LED 4K HDR Smart TV</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>